<commit_message>
wahrscheinlich was kapput gemacht ;)
</commit_message>
<xml_diff>
--- a/indikatoren.xlsx
+++ b/indikatoren.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaydi\Desktop\Projekt_2023\Projekt2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56A9130A-4F2B-407D-BE8F-EC0E71C8450A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1526417E-1C09-4056-B1F8-DD2FCC4CA3EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{B3B66726-B981-43AD-9244-AF1A9A2AEAE0}"/>
   </bookViews>
@@ -3704,7 +3704,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3757,12 +3757,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -3944,28 +3938,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
@@ -4317,8 +4311,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C6A5B6E-A67A-417D-B728-0D3FCA71EC49}">
   <dimension ref="A1:AO286"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A270" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P270" sqref="P270"/>
+    <sheetView tabSelected="1" topLeftCell="A269" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E270" sqref="E270"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Changed Scenario picker logic
</commit_message>
<xml_diff>
--- a/indikatoren.xlsx
+++ b/indikatoren.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaydi\Desktop\Projekt_2023\Projekt2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5C2307A-CBDE-4075-B0D3-A49F8EBC26D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1009F1F4-CFB8-4A7D-B98B-131FC1ED17C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{B3B66726-B981-43AD-9244-AF1A9A2AEAE0}"/>
   </bookViews>
@@ -4106,7 +4106,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4211,12 +4211,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -4431,7 +4425,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{CFDE625C-6074-4B64-A6A2-99F4C9AD683F}"/>
@@ -4772,8 +4766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C6A5B6E-A67A-417D-B728-0D3FCA71EC49}">
   <dimension ref="A1:BJ296"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="W4" sqref="W4"/>
+    <sheetView tabSelected="1" topLeftCell="A211" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AP211" sqref="AP211"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>